<commit_message>
Double checked all the 2pi coefficients and decay constant for STIRAP.jl Haven't modified the MonteCarlo one
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hu.sharepoint.com/sites/Yb/Shared Documents/Simulations/STIRAP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{5267DB95-DEB8-42EB-8863-1756DBEA282B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BB6CD5F-A7B7-426F-A690-4CBDF6BC861F}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{5267DB95-DEB8-42EB-8863-1756DBEA282B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{953D91AF-FE36-4B9C-BB60-23EBA3976ECC}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{E85E13B9-5144-4D4A-8D65-54A358140CE8}"/>
   </bookViews>
@@ -572,6 +572,3647 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$1:$A$461</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="461"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>132391.30429999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>164782.60870000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>197173.913</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>229565.21739999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>261956.52170000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>294347.82610000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>326739.13040000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>359130.43479999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>391521.73910000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>423913.04350000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>456304.34779999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>488695.65220000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>521086.95649999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>553478.26089999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>585869.56519999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>618260.86959999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>650652.17390000005</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>683043.47829999996</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>715434.78260000004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>747826.08700000006</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>780217.39130000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>812608.69570000004</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>845000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>877391.30429999996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>909782.60869999998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>942173.91299999994</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>974565.21739999996</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1006956.522</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1039347.826</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1071739.1299999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1104130.4350000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1136521.7390000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1168913.0430000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1201304.348</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1233695.652</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1266086.9569999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1298478.2609999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1330869.5649999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1363260.87</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1395652.1740000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1428043.4779999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1460434.7830000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1492826.0870000001</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1525217.3910000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1557608.696</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1590000</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1622391.304</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1654782.6089999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1687173.9129999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1719565.2169999999</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1751956.5220000001</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1784347.8259999999</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1816739.13</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1849130.4350000001</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1881521.7390000001</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1913913.0430000001</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1946304.348</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1978695.652</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2011086.9569999999</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2043478.2609999999</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2075869.5649999999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2108260.87</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2140652.1740000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2173043.4780000001</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2205434.7829999998</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2237826.0869999998</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2270217.3909999998</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2302608.696</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2335000</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2367391.304</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2399782.6090000002</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2432173.9130000002</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2464565.2170000002</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2496956.5219999999</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2529347.8259999999</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2561739.13</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2594130.4350000001</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2626521.7390000001</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2658913.0430000001</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2691304.3480000002</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2723695.6519999998</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2756086.9569999999</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2788478.2609999999</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2820869.5649999999</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2853260.87</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2885652.1740000001</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2918043.4780000001</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2950434.7829999998</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2982826.0869999998</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3015217.3909999998</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3047608.696</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3080000</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3112391.304</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3144782.6090000002</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3177173.9130000002</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3209565.2170000002</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3241956.5219999999</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3274347.8259999999</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3306739.13</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>3339130.4350000001</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>3371521.7390000001</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>3403913.0430000001</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>3436304.3480000002</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>3468695.6519999998</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>3501086.9569999999</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>3533478.2609999999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>3565869.5649999999</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>3598260.87</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>3630652.1740000001</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>3663043.4780000001</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>3695434.7829999998</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>3727826.0869999998</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>3760217.3909999998</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>3792608.696</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>3825000</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>3857391.304</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>3889782.6090000002</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>3922173.9130000002</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>3954565.2170000002</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>3986956.5219999999</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>4019347.8259999999</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>4051739.13</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>4084130.4350000001</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>4116521.7390000001</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>4148913.0430000001</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>4181304.3480000002</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>4213695.6519999998</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>4246086.9570000004</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>4278478.2609999999</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>4310869.5650000004</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>4343260.87</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>4375652.1739999996</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>4408043.4780000001</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>4440434.7829999998</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>4472826.0870000003</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>4505217.3909999998</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>4537608.6960000005</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>4570000</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>4602391.3039999995</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>4634782.6090000002</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>4667173.9129999997</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>4699565.2170000002</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>4731956.5219999999</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>4764347.8260000004</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>4796739.13</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>4829130.4349999996</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>4861521.7390000001</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>4893913.0429999996</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>4926304.3480000002</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>4958695.6519999998</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>4991086.9570000004</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>5023478.2609999999</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>5055869.5650000004</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>5088260.87</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>5120652.1739999996</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>5153043.4780000001</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>5185434.7829999998</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>5217826.0870000003</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>5250217.3909999998</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>5282608.6960000005</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>5315000</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>5347391.3039999995</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>5379782.6090000002</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>5412173.9129999997</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>5444565.2170000002</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>5476956.5219999999</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>5509347.8260000004</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>5541739.1299999999</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>5574130.4349999996</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>5606521.7390000001</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>5638913.0429999996</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>5671304.3480000002</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>5703695.6519999998</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>5736086.9570000004</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>5768478.2609999999</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>5800869.5650000004</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>5833260.8700000001</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>5865652.1739999996</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>5898043.4780000001</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>5930434.7829999998</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>5962826.0870000003</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>5995217.3909999998</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>6027608.6960000005</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>6060000</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>6092391.3039999995</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>6124782.6090000002</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>6157173.9129999997</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>6189565.2170000002</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>6221956.5219999999</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>6254347.8260000004</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>6286739.1299999999</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>6319130.4349999996</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>6351521.7390000001</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>6383913.0429999996</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>6416304.3480000002</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>6448695.6519999998</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>6481086.9570000004</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>6513478.2609999999</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>6545869.5650000004</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>6578260.8700000001</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>6610652.1739999996</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>6643043.4780000001</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>6675434.7829999998</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>6707826.0870000003</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>6740217.3909999998</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>6772608.6960000005</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>6805000</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>6837391.3039999995</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>6869782.6090000002</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>6902173.9129999997</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>6934565.2170000002</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>6966956.5219999999</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>6999347.8260000004</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>7031739.1299999999</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>7064130.4349999996</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>7096521.7390000001</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>7128913.0429999996</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>7161304.3480000002</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>7193695.6519999998</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>7226086.9570000004</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>7258478.2609999999</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>7290869.5650000004</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>7323260.8700000001</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>7355652.1739999996</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>7388043.4780000001</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>7420434.7829999998</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>7452826.0870000003</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>7485217.3909999998</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>7517608.6960000005</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>7550000</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>7582391.3039999995</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>7614782.6090000002</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>7647173.9129999997</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>7679565.2170000002</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>7711956.5219999999</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>7744347.8260000004</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>7776739.1299999999</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>7809130.4349999996</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>7841521.7390000001</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>7873913.0429999996</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>7906304.3480000002</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>7938695.6519999998</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>7971086.9570000004</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>8003478.2609999999</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>8035869.5650000004</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>8068260.8700000001</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>8100652.1739999996</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>8133043.4780000001</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>8165434.7829999998</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>8197826.0870000003</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>8230217.3909999998</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>8262608.6960000005</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>8295000</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>8327391.3039999995</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>8359782.6090000002</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>8392173.9130000006</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>8424565.2170000002</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>8456956.5219999999</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>8489347.8259999994</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>8521739.1300000008</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>8554130.4350000005</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>8586521.7390000001</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>8618913.0429999996</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>8651304.3479999993</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>8683695.6520000007</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>8716086.9570000004</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>8748478.2609999999</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>8780869.5649999995</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>8813260.8699999992</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>8845652.1740000006</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>8878043.4780000001</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>8910434.7829999998</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>8942826.0869999994</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>8975217.3910000008</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>9007608.6960000005</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>9040000</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>9072391.3039999995</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>9104782.6089999992</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>9137173.9130000006</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>9169565.2170000002</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>9201956.5219999999</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>9234347.8259999994</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>9266739.1300000008</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>9299130.4350000005</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>9331521.7390000001</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>9363913.0429999996</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>9396304.3479999993</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>9428695.6520000007</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>9461086.9570000004</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>9493478.2609999999</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>9525869.5649999995</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>9558260.8699999992</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>9590652.1740000006</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>9623043.4780000001</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>9655434.7829999998</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>9687826.0869999994</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>9720217.3910000008</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>9752608.6960000005</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>9785000</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>9817391.3039999995</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>9849782.6089999992</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>9882173.9130000006</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>9914565.2170000002</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>9946956.5219999999</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>9979347.8259999994</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>10011739.130000001</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>10044130.43</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>10076521.74</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>10108913.039999999</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>10141304.35</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>10173695.65</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>10206086.960000001</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>10238478.26</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>10270869.57</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>10303260.869999999</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>10335652.17</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>10368043.48</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>10400434.779999999</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>10432826.09</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>10465217.390000001</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>10497608.699999999</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>10530000</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>10562391.300000001</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>10594782.609999999</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>10627173.91</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>10659565.220000001</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>10691956.52</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>10724347.83</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>10756739.130000001</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>10789130.43</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>10821521.74</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>10853913.039999999</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>10886304.35</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>10918695.65</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>10951086.960000001</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>10983478.26</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>11015869.57</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>11048260.869999999</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>11080652.17</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>11113043.48</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>11145434.779999999</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>11177826.09</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>11210217.390000001</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>11242608.699999999</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>11275000</c:v>
+                </c:pt>
+                <c:pt idx="346">
+                  <c:v>11307391.300000001</c:v>
+                </c:pt>
+                <c:pt idx="347">
+                  <c:v>11339782.609999999</c:v>
+                </c:pt>
+                <c:pt idx="348">
+                  <c:v>11372173.91</c:v>
+                </c:pt>
+                <c:pt idx="349">
+                  <c:v>11404565.220000001</c:v>
+                </c:pt>
+                <c:pt idx="350">
+                  <c:v>11436956.52</c:v>
+                </c:pt>
+                <c:pt idx="351">
+                  <c:v>11469347.83</c:v>
+                </c:pt>
+                <c:pt idx="352">
+                  <c:v>11501739.130000001</c:v>
+                </c:pt>
+                <c:pt idx="353">
+                  <c:v>11534130.43</c:v>
+                </c:pt>
+                <c:pt idx="354">
+                  <c:v>11566521.74</c:v>
+                </c:pt>
+                <c:pt idx="355">
+                  <c:v>11598913.039999999</c:v>
+                </c:pt>
+                <c:pt idx="356">
+                  <c:v>11631304.35</c:v>
+                </c:pt>
+                <c:pt idx="357">
+                  <c:v>11663695.65</c:v>
+                </c:pt>
+                <c:pt idx="358">
+                  <c:v>11696086.960000001</c:v>
+                </c:pt>
+                <c:pt idx="359">
+                  <c:v>11728478.26</c:v>
+                </c:pt>
+                <c:pt idx="360">
+                  <c:v>11760869.57</c:v>
+                </c:pt>
+                <c:pt idx="361">
+                  <c:v>11793260.869999999</c:v>
+                </c:pt>
+                <c:pt idx="362">
+                  <c:v>11825652.17</c:v>
+                </c:pt>
+                <c:pt idx="363">
+                  <c:v>11858043.48</c:v>
+                </c:pt>
+                <c:pt idx="364">
+                  <c:v>11890434.779999999</c:v>
+                </c:pt>
+                <c:pt idx="365">
+                  <c:v>11922826.09</c:v>
+                </c:pt>
+                <c:pt idx="366">
+                  <c:v>11955217.390000001</c:v>
+                </c:pt>
+                <c:pt idx="367">
+                  <c:v>11987608.699999999</c:v>
+                </c:pt>
+                <c:pt idx="368">
+                  <c:v>12020000</c:v>
+                </c:pt>
+                <c:pt idx="369">
+                  <c:v>12052391.300000001</c:v>
+                </c:pt>
+                <c:pt idx="370">
+                  <c:v>12084782.609999999</c:v>
+                </c:pt>
+                <c:pt idx="371">
+                  <c:v>12117173.91</c:v>
+                </c:pt>
+                <c:pt idx="372">
+                  <c:v>12149565.220000001</c:v>
+                </c:pt>
+                <c:pt idx="373">
+                  <c:v>12181956.52</c:v>
+                </c:pt>
+                <c:pt idx="374">
+                  <c:v>12214347.83</c:v>
+                </c:pt>
+                <c:pt idx="375">
+                  <c:v>12246739.130000001</c:v>
+                </c:pt>
+                <c:pt idx="376">
+                  <c:v>12279130.43</c:v>
+                </c:pt>
+                <c:pt idx="377">
+                  <c:v>12311521.74</c:v>
+                </c:pt>
+                <c:pt idx="378">
+                  <c:v>12343913.039999999</c:v>
+                </c:pt>
+                <c:pt idx="379">
+                  <c:v>12376304.35</c:v>
+                </c:pt>
+                <c:pt idx="380">
+                  <c:v>12408695.65</c:v>
+                </c:pt>
+                <c:pt idx="381">
+                  <c:v>12441086.960000001</c:v>
+                </c:pt>
+                <c:pt idx="382">
+                  <c:v>12473478.26</c:v>
+                </c:pt>
+                <c:pt idx="383">
+                  <c:v>12505869.57</c:v>
+                </c:pt>
+                <c:pt idx="384">
+                  <c:v>12538260.869999999</c:v>
+                </c:pt>
+                <c:pt idx="385">
+                  <c:v>12570652.17</c:v>
+                </c:pt>
+                <c:pt idx="386">
+                  <c:v>12603043.48</c:v>
+                </c:pt>
+                <c:pt idx="387">
+                  <c:v>12635434.779999999</c:v>
+                </c:pt>
+                <c:pt idx="388">
+                  <c:v>12667826.09</c:v>
+                </c:pt>
+                <c:pt idx="389">
+                  <c:v>12700217.390000001</c:v>
+                </c:pt>
+                <c:pt idx="390">
+                  <c:v>12732608.699999999</c:v>
+                </c:pt>
+                <c:pt idx="391">
+                  <c:v>12765000</c:v>
+                </c:pt>
+                <c:pt idx="392">
+                  <c:v>12797391.300000001</c:v>
+                </c:pt>
+                <c:pt idx="393">
+                  <c:v>12829782.609999999</c:v>
+                </c:pt>
+                <c:pt idx="394">
+                  <c:v>12862173.91</c:v>
+                </c:pt>
+                <c:pt idx="395">
+                  <c:v>12894565.220000001</c:v>
+                </c:pt>
+                <c:pt idx="396">
+                  <c:v>12926956.52</c:v>
+                </c:pt>
+                <c:pt idx="397">
+                  <c:v>12959347.83</c:v>
+                </c:pt>
+                <c:pt idx="398">
+                  <c:v>12991739.130000001</c:v>
+                </c:pt>
+                <c:pt idx="399">
+                  <c:v>13024130.43</c:v>
+                </c:pt>
+                <c:pt idx="400">
+                  <c:v>13056521.74</c:v>
+                </c:pt>
+                <c:pt idx="401">
+                  <c:v>13088913.039999999</c:v>
+                </c:pt>
+                <c:pt idx="402">
+                  <c:v>13121304.35</c:v>
+                </c:pt>
+                <c:pt idx="403">
+                  <c:v>13153695.65</c:v>
+                </c:pt>
+                <c:pt idx="404">
+                  <c:v>13186086.960000001</c:v>
+                </c:pt>
+                <c:pt idx="405">
+                  <c:v>13218478.26</c:v>
+                </c:pt>
+                <c:pt idx="406">
+                  <c:v>13250869.57</c:v>
+                </c:pt>
+                <c:pt idx="407">
+                  <c:v>13283260.869999999</c:v>
+                </c:pt>
+                <c:pt idx="408">
+                  <c:v>13315652.17</c:v>
+                </c:pt>
+                <c:pt idx="409">
+                  <c:v>13348043.48</c:v>
+                </c:pt>
+                <c:pt idx="410">
+                  <c:v>13380434.779999999</c:v>
+                </c:pt>
+                <c:pt idx="411">
+                  <c:v>13412826.09</c:v>
+                </c:pt>
+                <c:pt idx="412">
+                  <c:v>13445217.390000001</c:v>
+                </c:pt>
+                <c:pt idx="413">
+                  <c:v>13477608.699999999</c:v>
+                </c:pt>
+                <c:pt idx="414">
+                  <c:v>13510000</c:v>
+                </c:pt>
+                <c:pt idx="415">
+                  <c:v>13542391.300000001</c:v>
+                </c:pt>
+                <c:pt idx="416">
+                  <c:v>13574782.609999999</c:v>
+                </c:pt>
+                <c:pt idx="417">
+                  <c:v>13607173.91</c:v>
+                </c:pt>
+                <c:pt idx="418">
+                  <c:v>13639565.220000001</c:v>
+                </c:pt>
+                <c:pt idx="419">
+                  <c:v>13671956.52</c:v>
+                </c:pt>
+                <c:pt idx="420">
+                  <c:v>13704347.83</c:v>
+                </c:pt>
+                <c:pt idx="421">
+                  <c:v>13736739.130000001</c:v>
+                </c:pt>
+                <c:pt idx="422">
+                  <c:v>13769130.43</c:v>
+                </c:pt>
+                <c:pt idx="423">
+                  <c:v>13801521.74</c:v>
+                </c:pt>
+                <c:pt idx="424">
+                  <c:v>13833913.039999999</c:v>
+                </c:pt>
+                <c:pt idx="425">
+                  <c:v>13866304.35</c:v>
+                </c:pt>
+                <c:pt idx="426">
+                  <c:v>13898695.65</c:v>
+                </c:pt>
+                <c:pt idx="427">
+                  <c:v>13931086.960000001</c:v>
+                </c:pt>
+                <c:pt idx="428">
+                  <c:v>13963478.26</c:v>
+                </c:pt>
+                <c:pt idx="429">
+                  <c:v>13995869.57</c:v>
+                </c:pt>
+                <c:pt idx="430">
+                  <c:v>14028260.869999999</c:v>
+                </c:pt>
+                <c:pt idx="431">
+                  <c:v>14060652.17</c:v>
+                </c:pt>
+                <c:pt idx="432">
+                  <c:v>14093043.48</c:v>
+                </c:pt>
+                <c:pt idx="433">
+                  <c:v>14125434.779999999</c:v>
+                </c:pt>
+                <c:pt idx="434">
+                  <c:v>14157826.09</c:v>
+                </c:pt>
+                <c:pt idx="435">
+                  <c:v>14190217.390000001</c:v>
+                </c:pt>
+                <c:pt idx="436">
+                  <c:v>14222608.699999999</c:v>
+                </c:pt>
+                <c:pt idx="437">
+                  <c:v>14255000</c:v>
+                </c:pt>
+                <c:pt idx="438">
+                  <c:v>14287391.300000001</c:v>
+                </c:pt>
+                <c:pt idx="439">
+                  <c:v>14319782.609999999</c:v>
+                </c:pt>
+                <c:pt idx="440">
+                  <c:v>14352173.91</c:v>
+                </c:pt>
+                <c:pt idx="441">
+                  <c:v>14384565.220000001</c:v>
+                </c:pt>
+                <c:pt idx="442">
+                  <c:v>14416956.52</c:v>
+                </c:pt>
+                <c:pt idx="443">
+                  <c:v>14449347.83</c:v>
+                </c:pt>
+                <c:pt idx="444">
+                  <c:v>14481739.130000001</c:v>
+                </c:pt>
+                <c:pt idx="445">
+                  <c:v>14514130.43</c:v>
+                </c:pt>
+                <c:pt idx="446">
+                  <c:v>14546521.74</c:v>
+                </c:pt>
+                <c:pt idx="447">
+                  <c:v>14578913.039999999</c:v>
+                </c:pt>
+                <c:pt idx="448">
+                  <c:v>14611304.35</c:v>
+                </c:pt>
+                <c:pt idx="449">
+                  <c:v>14643695.65</c:v>
+                </c:pt>
+                <c:pt idx="450">
+                  <c:v>14676086.960000001</c:v>
+                </c:pt>
+                <c:pt idx="451">
+                  <c:v>14708478.26</c:v>
+                </c:pt>
+                <c:pt idx="452">
+                  <c:v>14740869.57</c:v>
+                </c:pt>
+                <c:pt idx="453">
+                  <c:v>14773260.869999999</c:v>
+                </c:pt>
+                <c:pt idx="454">
+                  <c:v>14805652.17</c:v>
+                </c:pt>
+                <c:pt idx="455">
+                  <c:v>14838043.48</c:v>
+                </c:pt>
+                <c:pt idx="456">
+                  <c:v>14870434.779999999</c:v>
+                </c:pt>
+                <c:pt idx="457">
+                  <c:v>14902826.09</c:v>
+                </c:pt>
+                <c:pt idx="458">
+                  <c:v>14935217.390000001</c:v>
+                </c:pt>
+                <c:pt idx="459">
+                  <c:v>14967608.699999999</c:v>
+                </c:pt>
+                <c:pt idx="460">
+                  <c:v>15000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$1:$C$461</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="461"/>
+                <c:pt idx="0">
+                  <c:v>2.9361794381002783E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8674942818558797E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9709496241559133E-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7803482988849711E-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9381608120241821E-7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.3654134671091298E-7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5479562509075628E-7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0672775483096108E-7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.9652124641996114E-7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.6452901410016087E-7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.1603976241322487E-7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.8425690126810181E-7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.6374796473702072E-7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.0227536621443608E-7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.6854981204346873E-7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.6175462435911859E-7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.450669054612178E-7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.9731103737046215E-7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.6972524465859678E-7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.1196592722600416E-7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.0149729499063035E-6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.8026382621233291E-6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.6873400155412019E-6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.7200494343422837E-6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.5908300835956052E-6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.422971979222125E-6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.6292864167011201E-6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.9026462639379426E-6</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.0400690851289899E-6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.769611304657523E-6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.041338338700989E-6</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.026129384606002E-7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.2130405773736208E-7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.7470201621554347E-7</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.0863360169247841E-7</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.8987683843202737E-7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.5358507433944444E-7</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.3899131066785365E-7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9.082452285866326E-8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.190496782513454E-7</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.4005634708550362E-7</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6.7214468532746917E-8</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6.0318486949466998E-8</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.143195181502448E-8</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.9314348760186946E-8</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>6.4357488980190532E-8</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.4869730667335566E-8</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.4828170419502776E-8</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5.0476400667263707E-8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.7377221770251103E-8</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.9112786344726424E-8</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.1486688234117163E-8</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.434946300511607E-8</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.1309367388550739E-8</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.3297390597413561E-8</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.5052547834597101E-8</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.4013583661046292E-8</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.2876773602229739E-8</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.8424588215830628E-8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>6.8726715159120594E-7</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.2029275931798231E-8</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.4776432471198428E-8</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.7196031737803708E-8</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.1249704984577314E-8</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.8698908393694443E-8</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>9.7017050695404422E-9</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.1216972134775335E-8</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.2313448972811518E-8</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.1641423484042549E-8</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.1701653204035432E-8</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.4253048928275774E-8</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9.6565180585581143E-9</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>8.9105603097265273E-9</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>8.3900106479136225E-9</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>9.8958883787782733E-9</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>9.6064182878634732E-9</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.4208000345650856E-8</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>8.0266044217267253E-9</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6.0522546252592267E-9</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.3263034490221751E-8</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>6.4949800286008854E-9</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6.8529206318743599E-9</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>6.7699502933606492E-9</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1.0742435456416872E-8</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>7.0812862757370573E-9</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>6.9061570462935686E-9</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>5.909401567070446E-9</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>6.0697698770846107E-9</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>5.6187178231564613E-9</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>8.5947016200542654E-9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2.7978563255245308E-7</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>8.1508877070276143E-9</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5.7094976692171914E-9</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>4.8848192115649385E-9</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1.1254820604957975E-8</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3.0291804829745013E-8</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>4.5839473838066231E-9</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1.4302498503612671E-8</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>7.9227613085287938E-9</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>6.2726660098292933E-9</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>9.6828734746872963E-9</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>9.1306133858270527E-9</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>7.223426964030425E-9</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>5.0621145671035724E-9</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>7.0574046619359663E-9</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>7.0846458590279632E-9</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>5.3888210134820674E-9</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>6.0196117465877813E-9</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>7.4327290246962141E-9</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1.8739125898020483E-8</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>9.0335295180211063E-9</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>6.1033387357322095E-9</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>8.3584109139309025E-9</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>9.3812820218377885E-9</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>6.7560557087858747E-9</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1.203971978008611E-8</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>6.488377027806138E-9</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>7.9096264783616395E-9</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>7.4755559109969999E-9</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>8.4055821115316605E-9</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1.3782754293136362E-8</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>3.4066660228273216E-8</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1.0086557787294881E-8</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1.3769080943406228E-8</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1.0088808393540979E-8</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>8.5479481074100079E-9</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1.0790173103637178E-8</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>9.4870517810618549E-8</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>4.6247298090942445E-9</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>7.2394081771415245E-9</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>7.2531181169454832E-9</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>7.0102891424106046E-9</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>4.7669875645296152E-9</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>8.0676642873367569E-9</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>8.2785859294142328E-9</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>2.6313845837455017E-9</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>1.7452633229577963E-8</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>5.5217129017330369E-9</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>6.1521785475238664E-9</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>8.213428105703668E-9</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>5.6108811170454866E-9</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>3.810274532733406E-9</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>6.2269103622297988E-9</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>6.5285202870605859E-9</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>5.4615191527548515E-9</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>3.7197089270526876E-8</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>1.3584118579744808E-8</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>3.8138506138576433E-9</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>9.0073590112049153E-9</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>9.5112987262752325E-9</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>7.9471416324554442E-9</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>6.4103777303983979E-8</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>2.7640716780805473E-7</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>1.7258632376378238E-8</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>1.4424143753848998E-8</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>2.5231042550377484E-8</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>1.469484444066165E-8</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>2.1556190154473973E-8</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>1.9231847031745307E-8</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>5.2972599452210446E-9</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>6.6669809470931475E-9</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>1.044853873310982E-8</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>4.9317817025878956E-9</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>6.2461489283532802E-9</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>3.8085479695136119E-9</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>8.168956717602729E-9</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>7.4664474704110588E-9</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>5.8637868740909193E-9</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>5.0879873280008817E-9</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>4.1472451219873088E-9</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>5.3298886990073606E-9</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>3.2729797173941337E-9</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>7.7090327913187348E-9</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>6.0329031309816841E-9</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>6.6035937831616777E-9</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>9.0418886617442169E-9</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>6.6913808175487599E-9</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>5.7889112708737526E-9</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>6.8866637891688841E-9</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>5.4166204993242385E-9</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>8.0154445120060886E-9</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>1.0925196577731795E-8</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>9.9314903968333386E-7</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>1.4145414955470744E-8</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>1.2273355618134604E-8</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>1.0086894464798274E-8</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>1.1466676518891983E-8</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>7.49256875660471E-9</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>8.0280851279929366E-9</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>4.872404975427006E-8</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>9.0428735505025723E-9</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>7.4727198157074304E-9</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>5.0984110296029643E-9</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>4.8212752459072409E-9</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>6.8042052389626149E-9</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>6.5482305553904432E-9</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>4.9420329881680179E-9</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>4.9332981115867433E-9</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>1.4453326184429642E-8</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>4.2228363180314818E-9</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>5.0214784589071291E-9</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>6.2129077756874945E-9</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>5.0449096639243357E-9</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>4.0759130895691011E-9</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>5.9416972879339262E-9</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>5.4601233501218108E-9</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>6.1316134472587656E-9</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>5.0607674934417913E-9</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>6.8539620588924852E-9</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>1.0124352998917914E-8</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>1.2092404465893879E-8</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>1.8082092559462435E-8</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>1.2500617251724084E-8</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>1.5447900945069504E-6</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>1.0647630215619572E-8</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>5.9598976278266831E-9</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>7.5050373686715174E-9</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>1.5941274530884542E-8</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>5.4520624529432888E-9</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>4.2112683658112257E-9</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>7.9872547631296592E-9</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>8.6148667815626374E-9</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>7.7323750709367029E-9</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>3.278325591941214E-9</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>3.3724544376348175E-9</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>6.7264965688610096E-9</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>2.7517752550285508E-9</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>7.6129149856333132E-9</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>8.6227173441318738E-8</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>4.3872893107132662E-8</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>4.7207110226724062E-9</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>5.8587054751503506E-9</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>5.6990208650491826E-9</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>3.1356225280615269E-9</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>4.1138085834769968E-9</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>5.3408548969863632E-9</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>1.0728196832265265E-8</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>4.2030645027470217E-9</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>3.8417568738056104E-9</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>4.8036819919628773E-9</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>5.7841386264919135E-9</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>9.3173590369378895E-9</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>1.3220720138277275E-8</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>7.2074683673183728E-9</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>3.7012718396995917E-6</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>3.7275226234828374E-9</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>4.1919925485603175E-9</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>2.3793919503315908E-9</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>5.3892233650008811E-9</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>5.5431676144611537E-9</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>4.5998509460996088E-9</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>4.5961555043746102E-9</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>2.7629016959975218E-9</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>3.0533721426344224E-9</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>1.6410933513380211E-9</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>3.5212282950604613E-9</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>3.3397977592739107E-9</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>3.446612240036281E-9</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>3.374478263465219E-9</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>4.3288293748691905E-9</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>4.3923250581168669E-9</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>3.0654783975679177E-9</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>3.373171373343593E-9</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>2.9994842441889104E-9</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>1.916915958761404E-9</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>4.0774743244392478E-9</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>1.5165219268458262E-8</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>3.2698447263300376E-9</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>1.8331712985549982E-9</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>4.0618994828276598E-9</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>6.0424915117412596E-9</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>5.2063170154079716E-9</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>4.8805561654585109E-9</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>3.8396821337983066E-9</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>2.8155176746119062E-9</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>4.0649118490510493E-7</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>4.2228993750103875E-9</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>3.7988255735878563E-9</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>2.9176638064193232E-9</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>1.9547445547155726E-9</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>3.5797229084118695E-9</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>2.109603420748896E-9</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>6.7535281744694077E-9</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>4.8865701191662575E-9</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>1.1801509518411599E-8</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>2.1818766018464819E-9</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>2.9741124911114242E-9</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>5.2297470304980714E-9</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>2.4937081634404437E-9</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>5.8102200539862639E-9</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>2.5450867560066429E-9</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>3.6949701221324458E-9</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>5.4435066022745536E-9</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>3.4085606814445516E-9</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>3.6124593017795409E-9</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>2.9801819705496088E-9</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>5.7583462433348728E-9</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>1.4151753067254487E-7</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>2.9260818413244471E-9</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>2.0153119031600693E-9</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>3.5065921318954725E-9</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>3.3138024446952364E-9</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>2.932761618655295E-9</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>2.0053034408090154E-9</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>2.7778329877116569E-9</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>3.2798492430543263E-9</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>3.6577411399124478E-8</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>3.9066294170966983E-9</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>2.9063736002321334E-9</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>3.1584801293295354E-9</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>3.5430419707439866E-9</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>2.520685313365651E-9</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>1.933983951862063E-9</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>1.7349143131728584E-9</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>3.1591099616407017E-9</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>1.5509940187338289E-8</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>2.0136344700584391E-9</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>4.4450118694708066E-9</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>2.5521137301652385E-9</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>2.4890163876101085E-9</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>2.5426646078347961E-9</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>2.1325264378061108E-9</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>3.4364069127461997E-9</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>2.0013354353760091E-9</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>2.3134153665597926E-9</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>2.2327355122384834E-9</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>5.8859606182716964E-8</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>3.0151749406373159E-9</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>4.5095620703163273E-9</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>1.9109596895834118E-9</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>1.5879978679259155E-9</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>3.5314466687311861E-9</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>1.9577154715230778E-9</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>1.7917570171719201E-9</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>2.5042178334990752E-9</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>2.9373402337001188E-9</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>5.5337250642655231E-9</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>3.0283743841614705E-8</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>3.1143333539285783E-9</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>3.6008392345048643E-9</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>3.3342667072487736E-9</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>3.5301193034880271E-9</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>2.7675408502754276E-9</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>1.6524509838353224E-9</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>3.5092728223357798E-9</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>3.8000804063303041E-9</c:v>
+                </c:pt>
+                <c:pt idx="346">
+                  <c:v>3.6282989574002126E-9</c:v>
+                </c:pt>
+                <c:pt idx="347">
+                  <c:v>3.4297275972555313E-8</c:v>
+                </c:pt>
+                <c:pt idx="348">
+                  <c:v>4.7883563369940232E-9</c:v>
+                </c:pt>
+                <c:pt idx="349">
+                  <c:v>4.6272002847056819E-9</c:v>
+                </c:pt>
+                <c:pt idx="350">
+                  <c:v>1.9779644921434529E-9</c:v>
+                </c:pt>
+                <c:pt idx="351">
+                  <c:v>2.7471601118250761E-9</c:v>
+                </c:pt>
+                <c:pt idx="352">
+                  <c:v>2.0079102328030168E-9</c:v>
+                </c:pt>
+                <c:pt idx="353">
+                  <c:v>1.9765750771632596E-9</c:v>
+                </c:pt>
+                <c:pt idx="354">
+                  <c:v>4.7549646544366516E-9</c:v>
+                </c:pt>
+                <c:pt idx="355">
+                  <c:v>5.1400850609701113E-9</c:v>
+                </c:pt>
+                <c:pt idx="356">
+                  <c:v>3.2539318059518816E-9</c:v>
+                </c:pt>
+                <c:pt idx="357">
+                  <c:v>2.8063846871908876E-9</c:v>
+                </c:pt>
+                <c:pt idx="358">
+                  <c:v>2.1343854024140856E-9</c:v>
+                </c:pt>
+                <c:pt idx="359">
+                  <c:v>1.1141676153386545E-9</c:v>
+                </c:pt>
+                <c:pt idx="360">
+                  <c:v>5.4178481427887144E-9</c:v>
+                </c:pt>
+                <c:pt idx="361">
+                  <c:v>2.8854545171470719E-9</c:v>
+                </c:pt>
+                <c:pt idx="362">
+                  <c:v>2.6533873786387792E-9</c:v>
+                </c:pt>
+                <c:pt idx="363">
+                  <c:v>4.2139140094220111E-9</c:v>
+                </c:pt>
+                <c:pt idx="364">
+                  <c:v>5.6923320003277502E-9</c:v>
+                </c:pt>
+                <c:pt idx="365">
+                  <c:v>3.6342539237519804E-9</c:v>
+                </c:pt>
+                <c:pt idx="366">
+                  <c:v>3.8883142145873209E-9</c:v>
+                </c:pt>
+                <c:pt idx="367">
+                  <c:v>2.7536854002538508E-8</c:v>
+                </c:pt>
+                <c:pt idx="368">
+                  <c:v>3.1207081776414687E-7</c:v>
+                </c:pt>
+                <c:pt idx="369">
+                  <c:v>4.7492962095193187E-9</c:v>
+                </c:pt>
+                <c:pt idx="370">
+                  <c:v>3.1788646289424923E-9</c:v>
+                </c:pt>
+                <c:pt idx="371">
+                  <c:v>2.7639211551474726E-9</c:v>
+                </c:pt>
+                <c:pt idx="372">
+                  <c:v>4.8949814799605083E-9</c:v>
+                </c:pt>
+                <c:pt idx="373">
+                  <c:v>2.201145225233933E-9</c:v>
+                </c:pt>
+                <c:pt idx="374">
+                  <c:v>3.3873488401537738E-9</c:v>
+                </c:pt>
+                <c:pt idx="375">
+                  <c:v>2.6609213799501068E-9</c:v>
+                </c:pt>
+                <c:pt idx="376">
+                  <c:v>2.8252262841242908E-9</c:v>
+                </c:pt>
+                <c:pt idx="377">
+                  <c:v>4.0888040488675598E-9</c:v>
+                </c:pt>
+                <c:pt idx="378">
+                  <c:v>2.3188676133183831E-7</c:v>
+                </c:pt>
+                <c:pt idx="379">
+                  <c:v>2.975724755792853E-9</c:v>
+                </c:pt>
+                <c:pt idx="380">
+                  <c:v>4.7103850723086334E-9</c:v>
+                </c:pt>
+                <c:pt idx="381">
+                  <c:v>3.319774823432122E-9</c:v>
+                </c:pt>
+                <c:pt idx="382">
+                  <c:v>3.814091820084687E-9</c:v>
+                </c:pt>
+                <c:pt idx="383">
+                  <c:v>3.133086916320095E-9</c:v>
+                </c:pt>
+                <c:pt idx="384">
+                  <c:v>1.5752834271013686E-9</c:v>
+                </c:pt>
+                <c:pt idx="385">
+                  <c:v>3.4029545995232821E-9</c:v>
+                </c:pt>
+                <c:pt idx="386">
+                  <c:v>2.1332083697973605E-9</c:v>
+                </c:pt>
+                <c:pt idx="387">
+                  <c:v>2.093297317934869E-9</c:v>
+                </c:pt>
+                <c:pt idx="388">
+                  <c:v>3.1389403732638538E-9</c:v>
+                </c:pt>
+                <c:pt idx="389">
+                  <c:v>2.5382775462911141E-9</c:v>
+                </c:pt>
+                <c:pt idx="390">
+                  <c:v>2.0041887915275446E-9</c:v>
+                </c:pt>
+                <c:pt idx="391">
+                  <c:v>2.7627876373481818E-9</c:v>
+                </c:pt>
+                <c:pt idx="392">
+                  <c:v>2.6992003589549837E-9</c:v>
+                </c:pt>
+                <c:pt idx="393">
+                  <c:v>1.8072232077035586E-9</c:v>
+                </c:pt>
+                <c:pt idx="394">
+                  <c:v>4.6208763777597495E-9</c:v>
+                </c:pt>
+                <c:pt idx="395">
+                  <c:v>2.4744418315479201E-9</c:v>
+                </c:pt>
+                <c:pt idx="396">
+                  <c:v>3.1278899523564544E-9</c:v>
+                </c:pt>
+                <c:pt idx="397">
+                  <c:v>2.5590184967091596E-9</c:v>
+                </c:pt>
+                <c:pt idx="398">
+                  <c:v>9.6196834684577914E-7</c:v>
+                </c:pt>
+                <c:pt idx="399">
+                  <c:v>6.690070262931661E-9</c:v>
+                </c:pt>
+                <c:pt idx="400">
+                  <c:v>2.659524068451264E-9</c:v>
+                </c:pt>
+                <c:pt idx="401">
+                  <c:v>4.0986313254253052E-9</c:v>
+                </c:pt>
+                <c:pt idx="402">
+                  <c:v>2.2879951999329534E-9</c:v>
+                </c:pt>
+                <c:pt idx="403">
+                  <c:v>2.3677188898534314E-9</c:v>
+                </c:pt>
+                <c:pt idx="404">
+                  <c:v>3.5153936912179621E-9</c:v>
+                </c:pt>
+                <c:pt idx="405">
+                  <c:v>3.6974310586411138E-9</c:v>
+                </c:pt>
+                <c:pt idx="406">
+                  <c:v>3.6310535513200199E-9</c:v>
+                </c:pt>
+                <c:pt idx="407">
+                  <c:v>2.0556834431069517E-9</c:v>
+                </c:pt>
+                <c:pt idx="408">
+                  <c:v>2.2655014109861382E-9</c:v>
+                </c:pt>
+                <c:pt idx="409">
+                  <c:v>1.051919664859931E-7</c:v>
+                </c:pt>
+                <c:pt idx="410">
+                  <c:v>2.2822105728285925E-9</c:v>
+                </c:pt>
+                <c:pt idx="411">
+                  <c:v>2.6893861748704813E-9</c:v>
+                </c:pt>
+                <c:pt idx="412">
+                  <c:v>1.9406562175125408E-9</c:v>
+                </c:pt>
+                <c:pt idx="413">
+                  <c:v>1.8368736532376871E-9</c:v>
+                </c:pt>
+                <c:pt idx="414">
+                  <c:v>3.8548856960129849E-9</c:v>
+                </c:pt>
+                <c:pt idx="415">
+                  <c:v>1.3403983575403499E-9</c:v>
+                </c:pt>
+                <c:pt idx="416">
+                  <c:v>1.7681585686529821E-9</c:v>
+                </c:pt>
+                <c:pt idx="417">
+                  <c:v>2.0622230273515215E-9</c:v>
+                </c:pt>
+                <c:pt idx="418">
+                  <c:v>6.4608175355458969E-9</c:v>
+                </c:pt>
+                <c:pt idx="419">
+                  <c:v>3.2973483057923764E-9</c:v>
+                </c:pt>
+                <c:pt idx="420">
+                  <c:v>2.7214044524828702E-9</c:v>
+                </c:pt>
+                <c:pt idx="421">
+                  <c:v>4.1535847857394901E-9</c:v>
+                </c:pt>
+                <c:pt idx="422">
+                  <c:v>1.4240660109793076E-9</c:v>
+                </c:pt>
+                <c:pt idx="423">
+                  <c:v>1.3455320378164653E-9</c:v>
+                </c:pt>
+                <c:pt idx="424">
+                  <c:v>2.6668482622484699E-9</c:v>
+                </c:pt>
+                <c:pt idx="425">
+                  <c:v>3.0821288026733551E-9</c:v>
+                </c:pt>
+                <c:pt idx="426">
+                  <c:v>2.7620621338159765E-9</c:v>
+                </c:pt>
+                <c:pt idx="427">
+                  <c:v>2.0957055378164471E-9</c:v>
+                </c:pt>
+                <c:pt idx="428">
+                  <c:v>4.5901320541966975E-9</c:v>
+                </c:pt>
+                <c:pt idx="429">
+                  <c:v>2.5887342104305819E-7</c:v>
+                </c:pt>
+                <c:pt idx="430">
+                  <c:v>3.165123241811353E-9</c:v>
+                </c:pt>
+                <c:pt idx="431">
+                  <c:v>4.2645393980038999E-9</c:v>
+                </c:pt>
+                <c:pt idx="432">
+                  <c:v>4.4638824854384664E-9</c:v>
+                </c:pt>
+                <c:pt idx="433">
+                  <c:v>3.8355259111752537E-9</c:v>
+                </c:pt>
+                <c:pt idx="434">
+                  <c:v>3.3006140345340696E-9</c:v>
+                </c:pt>
+                <c:pt idx="435">
+                  <c:v>1.9699506109095267E-9</c:v>
+                </c:pt>
+                <c:pt idx="436">
+                  <c:v>2.0109407601404687E-9</c:v>
+                </c:pt>
+                <c:pt idx="437">
+                  <c:v>1.1041950782010044E-9</c:v>
+                </c:pt>
+                <c:pt idx="438">
+                  <c:v>2.187170602688927E-9</c:v>
+                </c:pt>
+                <c:pt idx="439">
+                  <c:v>1.8921992151080145E-9</c:v>
+                </c:pt>
+                <c:pt idx="440">
+                  <c:v>1.8575183168529043E-9</c:v>
+                </c:pt>
+                <c:pt idx="441">
+                  <c:v>1.9477021873989668E-8</c:v>
+                </c:pt>
+                <c:pt idx="442">
+                  <c:v>2.206102267469444E-9</c:v>
+                </c:pt>
+                <c:pt idx="443">
+                  <c:v>2.8791657208814119E-9</c:v>
+                </c:pt>
+                <c:pt idx="444">
+                  <c:v>1.6389469484736333E-9</c:v>
+                </c:pt>
+                <c:pt idx="445">
+                  <c:v>2.3136714204155739E-9</c:v>
+                </c:pt>
+                <c:pt idx="446">
+                  <c:v>2.7110141851800458E-9</c:v>
+                </c:pt>
+                <c:pt idx="447">
+                  <c:v>3.6264892047347733E-9</c:v>
+                </c:pt>
+                <c:pt idx="448">
+                  <c:v>3.0314349544006379E-8</c:v>
+                </c:pt>
+                <c:pt idx="449">
+                  <c:v>3.6690549325699779E-9</c:v>
+                </c:pt>
+                <c:pt idx="450">
+                  <c:v>2.2697499332582816E-9</c:v>
+                </c:pt>
+                <c:pt idx="451">
+                  <c:v>2.1356249894626802E-9</c:v>
+                </c:pt>
+                <c:pt idx="452">
+                  <c:v>2.4854531371830896E-9</c:v>
+                </c:pt>
+                <c:pt idx="453">
+                  <c:v>2.2075424977403981E-9</c:v>
+                </c:pt>
+                <c:pt idx="454">
+                  <c:v>3.832037214142509E-9</c:v>
+                </c:pt>
+                <c:pt idx="455">
+                  <c:v>2.3240999802725281E-9</c:v>
+                </c:pt>
+                <c:pt idx="456">
+                  <c:v>3.5117612227716845E-9</c:v>
+                </c:pt>
+                <c:pt idx="457">
+                  <c:v>3.2521288193148307E-9</c:v>
+                </c:pt>
+                <c:pt idx="458">
+                  <c:v>3.0820854908176887E-9</c:v>
+                </c:pt>
+                <c:pt idx="459">
+                  <c:v>2.8820729611240592E-9</c:v>
+                </c:pt>
+                <c:pt idx="460">
+                  <c:v>1.7963371681158142E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-39AC-4637-BB7D-FE30684F773A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1429232223"/>
+        <c:axId val="1429232703"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1429232223"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1429232703"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1429232703"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1429232223"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>212271</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>119744</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>185057</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>48987</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02741F34-F0F8-1217-7B58-FCDD2BA8D1C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -896,7 +4537,7 @@
   <dimension ref="A1:D461"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -8279,10 +11920,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="8bf5a133-002a-4534-987f-c92ee45a165d">
@@ -8291,15 +11942,6 @@
     <TaxCatchAll xmlns="e2c4e3f7-6411-4475-a680-21435a64b5a9" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8532,20 +12174,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C5F3E8E-2C13-43B0-AAC1-BB19DF90C74F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{860367E2-F27C-4BCD-8F13-7BEC0DEA7083}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="8bf5a133-002a-4534-987f-c92ee45a165d"/>
     <ds:schemaRef ds:uri="e2c4e3f7-6411-4475-a680-21435a64b5a9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C5F3E8E-2C13-43B0-AAC1-BB19DF90C74F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>